<commit_message>
Stack Stepdefs and PageObject
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -1,36 +1,87 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29203"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lingesh Raja\Documents\SDET\Dsalgo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DD14F5-289E-4BD0-9300-C4F1461F4182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{23D83EAA-3FBB-497B-A0B0-2BBC7A98EA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="3" r:id="rId1"/>
-    <sheet name="RegisterPage" sheetId="1" r:id="rId2"/>
-    <sheet name="LoginPageHoverText" sheetId="2" r:id="rId3"/>
-    <sheet name="LoginPageErrorMessage" sheetId="4" r:id="rId4"/>
+    <sheet name="TryEditor" sheetId="5" r:id="rId2"/>
+    <sheet name="RegisterPage" sheetId="1" r:id="rId3"/>
+    <sheet name="LoginPageHoverText" sheetId="2" r:id="rId4"/>
+    <sheet name="LoginPageErrorMessage" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="28">
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>tryCatchers@SDET</t>
+  </si>
+  <si>
+    <t>SDET@21389</t>
+  </si>
+  <si>
+    <t>InvalidCode</t>
+  </si>
+  <si>
+    <t>ValidCode</t>
+  </si>
+  <si>
+    <t>System.println(\"hello world\")</t>
+  </si>
+  <si>
+    <t>print(\"Hello\")</t>
+  </si>
+  <si>
+    <t>Password Confirmation</t>
+  </si>
+  <si>
+    <t>Error Message</t>
+  </si>
   <si>
     <t>SDET&amp;&amp;</t>
+  </si>
+  <si>
+    <t>sdfglkjh@24</t>
+  </si>
+  <si>
+    <t>Invalid Username</t>
+  </si>
+  <si>
+    <t>SDET$21,%</t>
   </si>
   <si>
     <r>
@@ -47,9 +98,6 @@
     </r>
   </si>
   <si>
-    <t>Invalid Username</t>
-  </si>
-  <si>
     <r>
       <t>SDET@</t>
     </r>
@@ -81,39 +129,21 @@
     <t>Invalid password</t>
   </si>
   <si>
-    <t>sdfglkjh@24</t>
+    <t>Test1234</t>
+  </si>
+  <si>
+    <t>sdfglkjh@2</t>
+  </si>
+  <si>
+    <t>password_mismatch:The two password fields didn’t match.</t>
   </si>
   <si>
     <t>User already registered</t>
   </si>
   <si>
-    <t>SDET$21,%</t>
-  </si>
-  <si>
-    <t>Test1234</t>
-  </si>
-  <si>
-    <t>sdfglkjh@2</t>
-  </si>
-  <si>
-    <t>password_mismatch:The two password fields didn’t match.</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>Field</t>
   </si>
   <si>
-    <t>Password Confirmation</t>
-  </si>
-  <si>
-    <t>Error Message</t>
-  </si>
-  <si>
     <t>SDETQA219</t>
   </si>
   <si>
@@ -127,19 +157,13 @@
   </si>
   <si>
     <t>SDE3890</t>
-  </si>
-  <si>
-    <t>tryCatchers@SDET</t>
-  </si>
-  <si>
-    <t>SDET@21389</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -508,29 +532,29 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="5" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="7" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -539,105 +563,137 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A79BDC4-EB22-400D-955E-F97D1F3E8F36}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="31.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="4" t="s">
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2">
         <v>2356789453</v>
@@ -646,61 +702,61 @@
         <v>2356789453</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1">
       <c r="A17" s="3"/>
     </row>
   </sheetData>
@@ -711,50 +767,50 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA5FB4FF-B525-479A-9EFD-46B2814FC312}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="C2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="B4" s="7" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -762,7 +818,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCF0593-1D3F-42D9-A724-6AF7A9C62239}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -770,45 +826,45 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C1" s="8"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C2" s="7"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified excelreader,config properties,config reader,test data,Hooks and Page object,step definitions and feature files for Home,Register,Launch,Login,Data Structures.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lingesh Raja\Documents\SDET\Dsalgo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lingesh Raja\git\Ds_AlGO_BDD\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DD14F5-289E-4BD0-9300-C4F1461F4182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEDA250-745E-4919-94D4-03BD50320E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="3" r:id="rId1"/>
-    <sheet name="RegisterPage" sheetId="1" r:id="rId2"/>
-    <sheet name="LoginPageHoverText" sheetId="2" r:id="rId3"/>
-    <sheet name="LoginPageErrorMessage" sheetId="4" r:id="rId4"/>
+    <sheet name="SuccessfulRegistration" sheetId="1" r:id="rId2"/>
+    <sheet name="TryEditor" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,111 +27,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
-  <si>
-    <t>SDET&amp;&amp;</t>
-  </si>
-  <si>
-    <r>
-      <t>sdfglkjh@</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF008000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>24</t>
-    </r>
-  </si>
-  <si>
-    <t>Invalid Username</t>
-  </si>
-  <si>
-    <r>
-      <t>SDET@</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF008000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>219</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>sjh@</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF008000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>24</t>
-    </r>
-  </si>
-  <si>
-    <t>Invalid password</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>sdfglkjh@24</t>
   </si>
   <si>
-    <t>User already registered</t>
-  </si>
-  <si>
-    <t>SDET$21,%</t>
-  </si>
-  <si>
-    <t>Test1234</t>
-  </si>
-  <si>
-    <t>sdfglkjh@2</t>
-  </si>
-  <si>
-    <t>password_mismatch:The two password fields didn’t match.</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
     <t>Password</t>
   </si>
   <si>
-    <t>Field</t>
-  </si>
-  <si>
     <t>Password Confirmation</t>
   </si>
   <si>
-    <t>Error Message</t>
-  </si>
-  <si>
     <t>SDETQA219</t>
   </si>
   <si>
-    <t>SA</t>
-  </si>
-  <si>
-    <t>SDET213890</t>
-  </si>
-  <si>
-    <t>SDET21389</t>
-  </si>
-  <si>
-    <t>SDE3890</t>
-  </si>
-  <si>
     <t>tryCatchers@SDET</t>
   </si>
   <si>
     <t>SDET@21389</t>
+  </si>
+  <si>
+    <t>ScenarioName</t>
+  </si>
+  <si>
+    <t>SuccessfulLogin</t>
+  </si>
+  <si>
+    <t>SuccessfulRegistration</t>
+  </si>
+  <si>
+    <t>InvalidCode</t>
+  </si>
+  <si>
+    <t>ValidCode</t>
+  </si>
+  <si>
+    <t>TryEditorValidation</t>
+  </si>
+  <si>
+    <t>System.println("hello world")</t>
+  </si>
+  <si>
+    <t>print("Hello")</t>
   </si>
 </sst>
 </file>
@@ -210,7 +149,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -222,8 +161,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -505,32 +442,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{358C323C-EFB0-421A-987A-331ECC3C90CA}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
-        <v>12</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>23</v>
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -543,12 +486,12 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="56.81640625" bestFit="1" customWidth="1"/>
@@ -556,134 +499,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
+      <c r="D2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="2">
-        <v>2356789453</v>
-      </c>
-      <c r="C7" s="2">
-        <v>2356789453</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
@@ -704,111 +585,43 @@
       <c r="A17" s="3"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" xr:uid="{B05EE001-5542-49FB-B047-5E503AAA3EB1}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA5FB4FF-B525-479A-9EFD-46B2814FC312}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09880E84-3817-4B86-8851-21FADE6B3A0D}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCF0593-1D3F-42D9-A724-6AF7A9C62239}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="7"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes part1 after review14Aug
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lingesh Raja\Documents\SDET\Dsalgo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23D83EAA-3FBB-497B-A0B0-2BBC7A98EA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9DC701A-569A-4E60-9D38-7BDEC46967CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="3" r:id="rId1"/>
@@ -60,10 +60,10 @@
     <t>ValidCode</t>
   </si>
   <si>
-    <t>System.println(\"hello world\")</t>
-  </si>
-  <si>
-    <t>print(\"Hello\")</t>
+    <t>System.println("hello world")</t>
+  </si>
+  <si>
+    <t>print("Hello")</t>
   </si>
   <si>
     <t>Password Confirmation</t>
@@ -567,7 +567,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>